<commit_message>
Atividade 3 Questão 4 - Solver
</commit_message>
<xml_diff>
--- a/Pesquisa_Operacional/Atividade_3_Questao_2.xlsx
+++ b/Pesquisa_Operacional/Atividade_3_Questao_2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repositories\Notas_Aulas_ESOF\Pesquisa_Operacional\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8D88B37-E3B3-42B0-8A2B-A88B4717EAE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEC66D7E-22DA-461B-8CE6-B74834A9C297}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2385" yWindow="3015" windowWidth="16710" windowHeight="10140" xr2:uid="{33388079-1998-4A9F-BCEA-2EE95CA90F9B}"/>
+    <workbookView xWindow="20310" yWindow="1890" windowWidth="16710" windowHeight="10140" xr2:uid="{33388079-1998-4A9F-BCEA-2EE95CA90F9B}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
     <definedName name="solver_itr" localSheetId="0" hidden="1">2147483647</definedName>
     <definedName name="solver_lhs1" localSheetId="0" hidden="1">Planilha1!$B$2:$D$2</definedName>
     <definedName name="solver_lhs2" localSheetId="0" hidden="1">Planilha1!$B$7:$B$8</definedName>
-    <definedName name="solver_lhs3" localSheetId="0" hidden="1">Planilha1!$B$9</definedName>
+    <definedName name="solver_lhs3" localSheetId="0" hidden="1">Planilha1!$B$9:$B$11</definedName>
     <definedName name="solver_lhs4" localSheetId="0" hidden="1">Planilha1!$B$2:$D$2</definedName>
     <definedName name="solver_lhs5" localSheetId="0" hidden="1">Planilha1!$B$7:$B$8</definedName>
     <definedName name="solver_mip" localSheetId="0" hidden="1">2147483647</definedName>
@@ -46,7 +46,7 @@
     <definedName name="solver_rel5" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_rhs1" localSheetId="0" hidden="1">"número inteiro"</definedName>
     <definedName name="solver_rhs2" localSheetId="0" hidden="1">Planilha1!$D$7:$D$8</definedName>
-    <definedName name="solver_rhs3" localSheetId="0" hidden="1">Planilha1!$D$9</definedName>
+    <definedName name="solver_rhs3" localSheetId="0" hidden="1">Planilha1!$D$9:$D$11</definedName>
     <definedName name="solver_rhs4" localSheetId="0" hidden="1">"número inteiro"</definedName>
     <definedName name="solver_rhs5" localSheetId="0" hidden="1">Planilha1!$D$7:$D$8</definedName>
     <definedName name="solver_rlx" localSheetId="0" hidden="1">2</definedName>
@@ -594,7 +594,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -619,10 +619,14 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B2" s="2">
-        <v>0</v>
-      </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
+        <v>10</v>
+      </c>
+      <c r="C2" s="2">
+        <v>11</v>
+      </c>
+      <c r="D2" s="2">
+        <v>56</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
@@ -630,7 +634,7 @@
       </c>
       <c r="B4">
         <f>350*B2+322*C2+355*D2</f>
-        <v>0</v>
+        <v>26922</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -644,7 +648,7 @@
       </c>
       <c r="B7" s="3">
         <f>0.7*B2+0.6*C2+0.65*D2</f>
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>17</v>
@@ -654,7 +658,7 @@
       </c>
       <c r="E7">
         <f>D7-B7</f>
-        <v>50</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -663,7 +667,7 @@
       </c>
       <c r="B8" s="3">
         <f>0.3*B2+0.35*C2+0.25*D2</f>
-        <v>0</v>
+        <v>20.85</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>17</v>
@@ -673,7 +677,7 @@
       </c>
       <c r="E8">
         <f t="shared" ref="E8:E11" si="0">D8-B8</f>
-        <v>35</v>
+        <v>14.149999999999999</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -682,7 +686,7 @@
       </c>
       <c r="B9" s="3">
         <f>B2</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>20</v>
@@ -692,7 +696,7 @@
       </c>
       <c r="E9">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -701,7 +705,7 @@
       </c>
       <c r="B10" s="3">
         <f>C2</f>
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>20</v>
@@ -711,7 +715,7 @@
       </c>
       <c r="E10">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>-4</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -720,7 +724,7 @@
       </c>
       <c r="B11" s="3">
         <f>D2</f>
-        <v>0</v>
+        <v>56</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>20</v>
@@ -730,7 +734,7 @@
       </c>
       <c r="E11">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>-45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>